<commit_message>
Dokonceni nadpisu "hluboke uceni" A stazeni "Machine Learning with Scikit Learn..."
</commit_message>
<xml_diff>
--- a/Tabulky/MapaUdaju.xlsx
+++ b/Tabulky/MapaUdaju.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ondra\Documents\VŠE\DP\Tabulky\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{772AEED6-08C8-4158-8375-CD1AC346C39E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{035C4ADD-37D7-4754-B1B7-4702704DDCB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-3576" windowWidth="30936" windowHeight="16896" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kompletní seznam" sheetId="1" r:id="rId1"/>

</xml_diff>